<commit_message>
A map legend to lasercut
The legend of the map ready to lasercut.
</commit_message>
<xml_diff>
--- a/Assignment 1/Data/cleanNicoledata.xlsx
+++ b/Assignment 1/Data/cleanNicoledata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Multec\Data Viz\DataVisualisation\Assignment 1\Data Cleaning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Multec\Data Viz\DataVisualisation\Assignment 1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC6CE5D-A484-4DAD-AEB9-11EE1ED7DD8B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044EAD09-546A-44C1-AE6A-C2E5D8C99979}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5004" xr2:uid="{F1E7017F-7F6C-4E68-82FF-E353ECF34D0C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2359" uniqueCount="1286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2360" uniqueCount="1287">
   <si>
     <t>11001</t>
   </si>
@@ -3888,6 +3888,9 @@
   </si>
   <si>
     <t>Luxemburg</t>
+  </si>
+  <si>
+    <t>Totaal</t>
   </si>
 </sst>
 </file>
@@ -4266,8 +4269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCCD21D-D897-4EF1-95B5-073070196799}">
   <dimension ref="A1:I615"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4578,6 +4581,13 @@
       <c r="E13">
         <v>45</v>
       </c>
+      <c r="H13" t="s">
+        <v>1286</v>
+      </c>
+      <c r="I13">
+        <f>SUM(I1:I11)</f>
+        <v>34520</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">

</xml_diff>